<commit_message>
added all changes done till now
</commit_message>
<xml_diff>
--- a/Forms/State forms/Central/Form V Muster Roll.xlsx
+++ b/Forms/State forms/Central/Form V Muster Roll.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>FORM V</t>
   </si>
@@ -61,6 +61,12 @@
   <si>
     <t>* Ins by G.S.R. 139, dated 16-1-1974 (w.e.f. 2-2-1974.)</t>
   </si>
+  <si>
+    <t>To:</t>
+  </si>
+  <si>
+    <t>From:</t>
+  </si>
 </sst>
 </file>
 
@@ -417,6 +423,39 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -433,39 +472,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -774,13 +780,13 @@
   <dimension ref="A1:AK13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C16" sqref="C16:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" style="2" customWidth="1"/>
     <col min="3" max="3" width="29" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="24.109375" style="2" customWidth="1"/>
@@ -794,213 +800,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="21"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="32"/>
     </row>
     <row r="2" spans="1:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="21"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
+      <c r="AF2" s="31"/>
+      <c r="AG2" s="31"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="32"/>
     </row>
     <row r="3" spans="1:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="20"/>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="20"/>
-      <c r="AD3" s="20"/>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
-      <c r="AH3" s="20"/>
-      <c r="AI3" s="20"/>
-      <c r="AJ3" s="20"/>
-      <c r="AK3" s="21"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="31"/>
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="31"/>
+      <c r="AG3" s="31"/>
+      <c r="AH3" s="31"/>
+      <c r="AI3" s="31"/>
+      <c r="AJ3" s="31"/>
+      <c r="AK3" s="32"/>
     </row>
     <row r="4" spans="1:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="23"/>
-      <c r="AH4" s="23"/>
-      <c r="AI4" s="23"/>
-      <c r="AJ4" s="23"/>
-      <c r="AK4" s="24"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="34"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="34"/>
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34"/>
+      <c r="AF4" s="34"/>
+      <c r="AG4" s="34"/>
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="34"/>
+      <c r="AJ4" s="34"/>
+      <c r="AK4" s="35"/>
     </row>
     <row r="5" spans="1:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
-      <c r="AD5" s="23"/>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="23"/>
-      <c r="AG5" s="23"/>
-      <c r="AH5" s="23"/>
-      <c r="AI5" s="23"/>
-      <c r="AJ5" s="23"/>
-      <c r="AK5" s="24"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="34"/>
+      <c r="AE5" s="34"/>
+      <c r="AF5" s="34"/>
+      <c r="AG5" s="34"/>
+      <c r="AH5" s="34"/>
+      <c r="AI5" s="34"/>
+      <c r="AJ5" s="34"/>
+      <c r="AK5" s="35"/>
     </row>
     <row r="6" spans="1:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
+      <c r="A6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>13</v>
+      </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -1038,64 +1048,64 @@
       <c r="AK6" s="18"/>
     </row>
     <row r="7" spans="1:37" s="13" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
-      <c r="AD7" s="26"/>
-      <c r="AE7" s="26"/>
-      <c r="AF7" s="26"/>
-      <c r="AG7" s="26"/>
-      <c r="AH7" s="26"/>
-      <c r="AI7" s="26"/>
-      <c r="AJ7" s="27"/>
-      <c r="AK7" s="28" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="21"/>
+      <c r="AK7" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:37" s="13" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="35"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="29"/>
       <c r="F8" s="12">
         <v>1</v>
       </c>
@@ -1189,7 +1199,7 @@
       <c r="AJ8" s="11">
         <v>31</v>
       </c>
-      <c r="AK8" s="29"/>
+      <c r="AK8" s="23"/>
     </row>
     <row r="9" spans="1:37" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
@@ -1390,6 +1400,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:AK1"/>
+    <mergeCell ref="A2:AK2"/>
+    <mergeCell ref="A3:AK3"/>
+    <mergeCell ref="A4:AK4"/>
+    <mergeCell ref="A5:AK5"/>
     <mergeCell ref="F7:AJ7"/>
     <mergeCell ref="AK7:AK8"/>
     <mergeCell ref="A7:A8"/>
@@ -1397,11 +1412,6 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A1:AK1"/>
-    <mergeCell ref="A2:AK2"/>
-    <mergeCell ref="A3:AK3"/>
-    <mergeCell ref="A4:AK4"/>
-    <mergeCell ref="A5:AK5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>